<commit_message>
passAtk, pickUpChar/Equip 작업용 엑셀 올림
</commit_message>
<xml_diff>
--- a/Excel/작업Gacha.xlsx
+++ b/Excel/작업Gacha.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNameless\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18D714E-CAE7-481A-B3B7-8E1ED7F768F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4313D81-6F55-4BBD-A6F1-C62DD972F939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{09274F9C-5D79-4C8F-9B53-4C593F8D4943}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="2" activeTab="7" xr2:uid="{09274F9C-5D79-4C8F-9B53-4C593F8D4943}"/>
   </bookViews>
   <sheets>
     <sheet name="GachaSpellTable" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="ShopActorTable" sheetId="6" r:id="rId4"/>
     <sheet name="ShopEquipTable" sheetId="5" r:id="rId5"/>
     <sheet name="GachaEquipTable" sheetId="3" r:id="rId6"/>
+    <sheet name="픽업캐릭" sheetId="7" r:id="rId7"/>
+    <sheet name="픽업이큅" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
   <si>
     <t>grade|Int</t>
   </si>
@@ -205,6 +207,108 @@
   </si>
   <si>
     <t>Equip20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>em</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시작일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종료일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Actor0201</t>
+  </si>
+  <si>
+    <t>Actor2238</t>
+  </si>
+  <si>
+    <t>참고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pickUpChar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>간파울</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관통</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pickUpEquip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Equip031201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ssc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ov</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Equip034201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Equip033001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -212,7 +316,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +337,28 @@
       <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -259,18 +385,41 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -584,7 +733,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
     <col min="3" max="3" width="28.75" customWidth="1"/>
     <col min="4" max="17" width="9" hidden="1" customWidth="1" outlineLevel="1"/>
@@ -593,7 +742,7 @@
     <col min="20" max="20" width="9" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="27" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -649,7 +798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1</v>
       </c>
@@ -709,7 +858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>1</v>
       </c>
@@ -773,7 +922,7 @@
         <v>1, 5, 10, 20, 40, 70, 110, 160, 210, 270, 340, 420, 510, 600</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>1</v>
       </c>
@@ -827,7 +976,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>0</v>
       </c>
@@ -881,7 +1030,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>0</v>
       </c>
@@ -935,7 +1084,7 @@
         <v>0.19700000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>0</v>
       </c>
@@ -989,7 +1138,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>0</v>
       </c>
@@ -1043,7 +1192,7 @@
         <v>0.24099999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" hidden="1" outlineLevel="1">
       <c r="C9" t="s">
         <v>5</v>
       </c>
@@ -1104,7 +1253,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:19" collapsed="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:19" collapsed="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1120,14 +1269,14 @@
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="9" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="27" customHeight="1">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1147,7 +1296,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1172,7 +1321,7 @@
         <v>{"2":5,"10":22,"50":100}</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1191,7 +1340,7 @@
         <v>"10":22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1224,13 +1373,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" outlineLevelCol="1"/>
   <cols>
     <col min="3" max="3" width="46.375" customWidth="1"/>
     <col min="4" max="24" width="9" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="27" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1304,7 +1453,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1383,7 +1532,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1462,7 +1611,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1556,14 +1705,14 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="9" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="27" customHeight="1">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1583,7 +1732,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1608,7 +1757,7 @@
         <v>{"1":15,"10":120}</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1638,18 +1787,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD48CC8-8B1A-494D-9B5E-6343713E47F3}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="9" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="27" customHeight="1">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1669,7 +1818,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1694,7 +1843,7 @@
         <v>{"1":20,"10":175,"20":300}</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1713,7 +1862,7 @@
         <v>"10":175</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1746,9 +1895,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="27" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1759,7 +1908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1770,7 +1919,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1781,7 +1930,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1792,7 +1941,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1803,7 +1952,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1814,7 +1963,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1829,4 +1978,609 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2E4E2B-4701-4F06-BDB0-D365FEE0C64E}">
+  <dimension ref="A1:R4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="16.75" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.875" style="4" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="12.625" customWidth="1"/>
+    <col min="11" max="11" width="9.875" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.625" customWidth="1"/>
+    <col min="14" max="14" width="5.5" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="16" width="9" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="9" customWidth="1" outlineLevel="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="27" customHeight="1">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2">
+        <f>YEAR(H2)</f>
+        <v>2023</v>
+      </c>
+      <c r="C2">
+        <f>MONTH(H2)</f>
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <f>DAY(H2)</f>
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <f>YEAR(I2+1)</f>
+        <v>2023</v>
+      </c>
+      <c r="F2">
+        <f>MONTH(I2+1)</f>
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <f>DAY(I2+1)</f>
+        <v>20</v>
+      </c>
+      <c r="H2" s="5">
+        <v>44967</v>
+      </c>
+      <c r="I2" s="5">
+        <v>44976</v>
+      </c>
+      <c r="J2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2">
+        <v>50</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+      <c r="M2">
+        <v>120</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" t="str">
+        <f t="shared" ref="O2" ca="1" si="0">IF(ROW()=2,P2,OFFSET(O2,-1,0)&amp;IF(LEN(P2)=0,"",","&amp;P2))</f>
+        <v>{"sy":"2023","sm":"2","sd":"10","ey":"2023","em":"2","ed":"20","id":"Actor0201","bc":50,"count":10,"price":120}</v>
+      </c>
+      <c r="P2" t="str">
+        <f>IF(N2&lt;&gt;1,"",
+"{"""&amp;B$1&amp;""":"""&amp;B2&amp;""""
+&amp;","""&amp;C$1&amp;""":"""&amp;C2&amp;""""
+&amp;","""&amp;D$1&amp;""":"""&amp;D2&amp;""""
+&amp;","""&amp;E$1&amp;""":"""&amp;E2&amp;""""
+&amp;","""&amp;F$1&amp;""":"""&amp;F2&amp;""""
+&amp;","""&amp;G$1&amp;""":"""&amp;G2&amp;""""
+&amp;IF(LEN(J2)=0,"",","""&amp;J$1&amp;""":"""&amp;J2&amp;"""")
+&amp;IF(LEN(K2)=0,"",","""&amp;K$1&amp;""":"&amp;K2)
+&amp;IF(LEN(L2)=0,"",","""&amp;L$1&amp;""":"&amp;L2)
+&amp;IF(LEN(M2)=0,"",","""&amp;M$1&amp;""":"&amp;M2)&amp;"}")</f>
+        <v>{"sy":"2023","sm":"2","sd":"10","ey":"2023","em":"2","ed":"20","id":"Actor0201","bc":50,"count":10,"price":120}</v>
+      </c>
+      <c r="R2" t="str">
+        <f ca="1">"["&amp;
+IF(LEFT(OFFSET(O1,COUNTA(O:O)-1,0),1)=",",SUBSTITUTE(OFFSET(O1,COUNTA(O:O)-1,0),",","",1),OFFSET(O1,COUNTA(O:O)-1,0))
+&amp;"]"</f>
+        <v>[{"sy":"2023","sm":"2","sd":"10","ey":"2023","em":"2","ed":"20","id":"Actor0201","bc":50,"count":10,"price":120},{"sy":"2023","sm":"2","sd":"25","ey":"2023","em":"3","ed":"5","id":"Actor0201","bc":50,"count":10,"price":120},{"sy":"2023","sm":"3","sd":"5","ey":"2023","em":"3","ed":"12","id":"Actor2238","bc":50,"count":10,"price":120}]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B4" si="1">YEAR(H3)</f>
+        <v>2023</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C4" si="2">MONTH(H3)</f>
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D4" si="3">DAY(H3)</f>
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E4" si="4">YEAR(I3+1)</f>
+        <v>2023</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F4" si="5">MONTH(I3+1)</f>
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G4" si="6">DAY(I3+1)</f>
+        <v>5</v>
+      </c>
+      <c r="H3" s="5">
+        <v>44982</v>
+      </c>
+      <c r="I3" s="5">
+        <v>44989</v>
+      </c>
+      <c r="J3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3">
+        <v>50</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+      <c r="M3">
+        <v>120</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O4" ca="1" si="7">IF(ROW()=2,P3,OFFSET(O3,-1,0)&amp;IF(LEN(P3)=0,"",","&amp;P3))</f>
+        <v>{"sy":"2023","sm":"2","sd":"10","ey":"2023","em":"2","ed":"20","id":"Actor0201","bc":50,"count":10,"price":120},{"sy":"2023","sm":"2","sd":"25","ey":"2023","em":"3","ed":"5","id":"Actor0201","bc":50,"count":10,"price":120}</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" ref="P3:P4" si="8">IF(N3&lt;&gt;1,"",
+"{"""&amp;B$1&amp;""":"""&amp;B3&amp;""""
+&amp;","""&amp;C$1&amp;""":"""&amp;C3&amp;""""
+&amp;","""&amp;D$1&amp;""":"""&amp;D3&amp;""""
+&amp;","""&amp;E$1&amp;""":"""&amp;E3&amp;""""
+&amp;","""&amp;F$1&amp;""":"""&amp;F3&amp;""""
+&amp;","""&amp;G$1&amp;""":"""&amp;G3&amp;""""
+&amp;IF(LEN(J3)=0,"",","""&amp;J$1&amp;""":"""&amp;J3&amp;"""")
+&amp;IF(LEN(K3)=0,"",","""&amp;K$1&amp;""":"&amp;K3)
+&amp;IF(LEN(L3)=0,"",","""&amp;L$1&amp;""":"&amp;L3)
+&amp;IF(LEN(M3)=0,"",","""&amp;M$1&amp;""":"&amp;M3)&amp;"}")</f>
+        <v>{"sy":"2023","sm":"2","sd":"25","ey":"2023","em":"3","ed":"5","id":"Actor0201","bc":50,"count":10,"price":120}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="1"/>
+        <v>2023</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="H4" s="5">
+        <v>44990</v>
+      </c>
+      <c r="I4" s="5">
+        <v>44996</v>
+      </c>
+      <c r="J4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4">
+        <v>50</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4">
+        <v>120</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>{"sy":"2023","sm":"2","sd":"10","ey":"2023","em":"2","ed":"20","id":"Actor0201","bc":50,"count":10,"price":120},{"sy":"2023","sm":"2","sd":"25","ey":"2023","em":"3","ed":"5","id":"Actor0201","bc":50,"count":10,"price":120},{"sy":"2023","sm":"3","sd":"5","ey":"2023","em":"3","ed":"12","id":"Actor2238","bc":50,"count":10,"price":120}</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="8"/>
+        <v>{"sy":"2023","sm":"3","sd":"5","ey":"2023","em":"3","ed":"12","id":"Actor2238","bc":50,"count":10,"price":120}</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="H1:I1048576">
+    <cfRule type="expression" dxfId="1" priority="5">
+      <formula>OR($N1=0,$I1&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D2961BD-E0AE-4D3B-B718-993382D622B5}">
+  <dimension ref="A1:T4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T2" sqref="T2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="16.75" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.875" style="4" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="12.625" customWidth="1"/>
+    <col min="11" max="12" width="4.625" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="6.625" customWidth="1"/>
+    <col min="16" max="16" width="5.5" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="18" width="9" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="9" customWidth="1" outlineLevel="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="27" customHeight="1">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="B2">
+        <f>YEAR(H2)</f>
+        <v>2023</v>
+      </c>
+      <c r="C2">
+        <f>MONTH(H2)</f>
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <f>DAY(H2)</f>
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <f>YEAR(I2+1)</f>
+        <v>2023</v>
+      </c>
+      <c r="F2">
+        <f>MONTH(I2+1)</f>
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <f>DAY(I2+1)</f>
+        <v>22</v>
+      </c>
+      <c r="H2" s="5">
+        <v>44967</v>
+      </c>
+      <c r="I2" s="5">
+        <v>44978</v>
+      </c>
+      <c r="J2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2">
+        <v>50</v>
+      </c>
+      <c r="L2">
+        <v>100</v>
+      </c>
+      <c r="M2">
+        <v>20</v>
+      </c>
+      <c r="N2">
+        <v>300</v>
+      </c>
+      <c r="O2">
+        <v>0.02</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="str">
+        <f t="shared" ref="Q2:Q4" ca="1" si="0">IF(ROW()=2,R2,OFFSET(Q2,-1,0)&amp;IF(LEN(R2)=0,"",","&amp;R2))</f>
+        <v>{"sy":"2023","sm":"2","sd":"10","ey":"2023","em":"2","ed":"22","id":"Equip031201","sc":50,"ssc":100,"count":20,"price":300,"ov":0.02}</v>
+      </c>
+      <c r="R2" t="str">
+        <f>IF(P2&lt;&gt;1,"",
+"{"""&amp;B$1&amp;""":"""&amp;B2&amp;""""
+&amp;","""&amp;C$1&amp;""":"""&amp;C2&amp;""""
+&amp;","""&amp;D$1&amp;""":"""&amp;D2&amp;""""
+&amp;","""&amp;E$1&amp;""":"""&amp;E2&amp;""""
+&amp;","""&amp;F$1&amp;""":"""&amp;F2&amp;""""
+&amp;","""&amp;G$1&amp;""":"""&amp;G2&amp;""""
+&amp;IF(LEN(J2)=0,"",","""&amp;J$1&amp;""":"""&amp;J2&amp;"""")
+&amp;IF(LEN(K2)=0,"",","""&amp;K$1&amp;""":"&amp;K2)
+&amp;IF(LEN(L2)=0,"",","""&amp;L$1&amp;""":"&amp;L2)
+&amp;IF(LEN(M2)=0,"",","""&amp;M$1&amp;""":"&amp;M2)
+&amp;IF(LEN(N2)=0,"",","""&amp;N$1&amp;""":"&amp;N2)
+&amp;IF(LEN(O2)=0,"",","""&amp;O$1&amp;""":"&amp;O2)&amp;"}")</f>
+        <v>{"sy":"2023","sm":"2","sd":"10","ey":"2023","em":"2","ed":"22","id":"Equip031201","sc":50,"ssc":100,"count":20,"price":300,"ov":0.02}</v>
+      </c>
+      <c r="T2" t="str">
+        <f ca="1">"["&amp;
+IF(LEFT(OFFSET(Q1,COUNTA(Q:Q)-1,0),1)=",",SUBSTITUTE(OFFSET(Q1,COUNTA(Q:Q)-1,0),",","",1),OFFSET(Q1,COUNTA(Q:Q)-1,0))
+&amp;"]"</f>
+        <v>[{"sy":"2023","sm":"2","sd":"10","ey":"2023","em":"2","ed":"22","id":"Equip031201","sc":50,"ssc":100,"count":20,"price":300,"ov":0.02},{"sy":"2023","sm":"2","sd":"23","ey":"2023","em":"3","ed":"7","id":"Equip034201","sc":50,"ssc":100,"count":20,"price":300,"ov":0.02},{"sy":"2023","sm":"3","sd":"5","ey":"2023","em":"3","ed":"15","id":"Equip033001","sc":50,"ssc":100,"count":20,"price":300,"ov":0.02}]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="B3">
+        <f t="shared" ref="B3:B4" si="1">YEAR(H3)</f>
+        <v>2023</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C4" si="2">MONTH(H3)</f>
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D4" si="3">DAY(H3)</f>
+        <v>23</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E4" si="4">YEAR(I3+1)</f>
+        <v>2023</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F4" si="5">MONTH(I3+1)</f>
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G4" si="6">DAY(I3+1)</f>
+        <v>7</v>
+      </c>
+      <c r="H3" s="5">
+        <v>44980</v>
+      </c>
+      <c r="I3" s="5">
+        <v>44991</v>
+      </c>
+      <c r="J3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3">
+        <v>50</v>
+      </c>
+      <c r="L3">
+        <v>100</v>
+      </c>
+      <c r="M3">
+        <v>20</v>
+      </c>
+      <c r="N3">
+        <v>300</v>
+      </c>
+      <c r="O3">
+        <v>0.02</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>{"sy":"2023","sm":"2","sd":"10","ey":"2023","em":"2","ed":"22","id":"Equip031201","sc":50,"ssc":100,"count":20,"price":300,"ov":0.02},{"sy":"2023","sm":"2","sd":"23","ey":"2023","em":"3","ed":"7","id":"Equip034201","sc":50,"ssc":100,"count":20,"price":300,"ov":0.02}</v>
+      </c>
+      <c r="R3" t="str">
+        <f t="shared" ref="R3:R4" si="7">IF(P3&lt;&gt;1,"",
+"{"""&amp;B$1&amp;""":"""&amp;B3&amp;""""
+&amp;","""&amp;C$1&amp;""":"""&amp;C3&amp;""""
+&amp;","""&amp;D$1&amp;""":"""&amp;D3&amp;""""
+&amp;","""&amp;E$1&amp;""":"""&amp;E3&amp;""""
+&amp;","""&amp;F$1&amp;""":"""&amp;F3&amp;""""
+&amp;","""&amp;G$1&amp;""":"""&amp;G3&amp;""""
+&amp;IF(LEN(J3)=0,"",","""&amp;J$1&amp;""":"""&amp;J3&amp;"""")
+&amp;IF(LEN(K3)=0,"",","""&amp;K$1&amp;""":"&amp;K3)
+&amp;IF(LEN(L3)=0,"",","""&amp;L$1&amp;""":"&amp;L3)
+&amp;IF(LEN(M3)=0,"",","""&amp;M$1&amp;""":"&amp;M3)
+&amp;IF(LEN(N3)=0,"",","""&amp;N$1&amp;""":"&amp;N3)
+&amp;IF(LEN(O3)=0,"",","""&amp;O$1&amp;""":"&amp;O3)&amp;"}")</f>
+        <v>{"sy":"2023","sm":"2","sd":"23","ey":"2023","em":"3","ed":"7","id":"Equip034201","sc":50,"ssc":100,"count":20,"price":300,"ov":0.02}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="B4">
+        <f t="shared" si="1"/>
+        <v>2023</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="H4" s="5">
+        <v>44990</v>
+      </c>
+      <c r="I4" s="5">
+        <v>44999</v>
+      </c>
+      <c r="J4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4">
+        <v>50</v>
+      </c>
+      <c r="L4">
+        <v>100</v>
+      </c>
+      <c r="M4">
+        <v>20</v>
+      </c>
+      <c r="N4">
+        <v>300</v>
+      </c>
+      <c r="O4">
+        <v>0.02</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>{"sy":"2023","sm":"2","sd":"10","ey":"2023","em":"2","ed":"22","id":"Equip031201","sc":50,"ssc":100,"count":20,"price":300,"ov":0.02},{"sy":"2023","sm":"2","sd":"23","ey":"2023","em":"3","ed":"7","id":"Equip034201","sc":50,"ssc":100,"count":20,"price":300,"ov":0.02},{"sy":"2023","sm":"3","sd":"5","ey":"2023","em":"3","ed":"15","id":"Equip033001","sc":50,"ssc":100,"count":20,"price":300,"ov":0.02}</v>
+      </c>
+      <c r="R4" t="str">
+        <f t="shared" si="7"/>
+        <v>{"sy":"2023","sm":"3","sd":"5","ey":"2023","em":"3","ed":"15","id":"Equip033001","sc":50,"ssc":100,"count":20,"price":300,"ov":0.02}</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="H1:I1048576">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>OR($P1=0,$I1&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>